<commit_message>
minor fix mobile + text
</commit_message>
<xml_diff>
--- a/test.xlsx
+++ b/test.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24931"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25028"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="O:\халтура\Pablo Hookahbar\Pablo-hookahbar\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4797C4D6-2410-4024-8493-139BFC360777}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8F2BCA5F-02EC-45B8-B1BA-3A4C196F4E53}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="9555" yWindow="4215" windowWidth="19245" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Лист1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="428" uniqueCount="372">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="433" uniqueCount="377">
   <si>
     <t>Назание</t>
   </si>
@@ -1145,6 +1145,21 @@
   </si>
   <si>
     <t>Киликия.jpg</t>
+  </si>
+  <si>
+    <t>Зеленый чай с имбирем, корицей и медом, корень имбиря, лимон</t>
+  </si>
+  <si>
+    <t>Фруктовый чай (на основе черного), клубничный десерт, клубника, маракуйя</t>
+  </si>
+  <si>
+    <t>Фруктовый чай (на основе черного), клубничный десерт, малина</t>
+  </si>
+  <si>
+    <t>Черный облепиховый чай, облепиха, имбирь</t>
+  </si>
+  <si>
+    <t>Черный индийский чай с пряностями (корица, анис, гвоздика, имбирь, кориандр, чёрный перец, кардамон, тмин), молоко, мед</t>
   </si>
 </sst>
 </file>
@@ -1558,8 +1573,8 @@
   <dimension ref="A1:F431"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A116" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C139" sqref="C139"/>
+      <pane ySplit="1" topLeftCell="A17" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E41" sqref="E41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2226,7 +2241,9 @@
       <c r="E40" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="F40" s="3"/>
+      <c r="F40" s="3" t="s">
+        <v>376</v>
+      </c>
     </row>
     <row r="41" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A41" s="2"/>
@@ -2242,7 +2259,9 @@
       <c r="E41" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="F41" s="3"/>
+      <c r="F41" s="3" t="s">
+        <v>375</v>
+      </c>
     </row>
     <row r="42" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A42" s="2"/>
@@ -2258,7 +2277,9 @@
       <c r="E42" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="F42" s="3"/>
+      <c r="F42" s="3" t="s">
+        <v>372</v>
+      </c>
     </row>
     <row r="43" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A43" s="2"/>
@@ -2274,7 +2295,9 @@
       <c r="E43" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="F43" s="3"/>
+      <c r="F43" s="3" t="s">
+        <v>374</v>
+      </c>
     </row>
     <row r="44" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A44" s="2"/>
@@ -2290,7 +2313,9 @@
       <c r="E44" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="F44" s="3"/>
+      <c r="F44" s="3" t="s">
+        <v>373</v>
+      </c>
     </row>
     <row r="45" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A45" s="8" t="s">

</xml_diff>